<commit_message>
Add review comments to all templates
</commit_message>
<xml_diff>
--- a/templates/2EXT01_RNA/2EXT01_RNA.xlsx
+++ b/templates/2EXT01_RNA/2EXT01_RNA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Google Drive/CEPLAS/MetadataTemplates/SWATE_templates/templates/2EXT01_RNA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\nfdi4plants\SWATE_templates\templates\2EXT01_RNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776E2BBA-D2F3-3B49-8DAE-7854A514061F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDC9B7E-89E2-49D8-A7D9-C4472F5C5A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4720" yWindow="-21100" windowWidth="39240" windowHeight="21100" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
   </bookViews>
   <sheets>
     <sheet name="2EXT01_RNA" sheetId="3" r:id="rId1"/>
@@ -20,12 +20,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="103">
   <si>
     <t>Source Name</t>
   </si>
@@ -321,6 +330,24 @@
   <si>
     <t>Include one of the following: total RNA, polyA RNA, cytoplasmic RNA, nuclear RNA, genomic DNA, protein, or other.</t>
   </si>
+  <si>
+    <t>The name of the output of this assay</t>
+  </si>
+  <si>
+    <t>User instruction missing</t>
+  </si>
+  <si>
+    <t>Do we want to give a unit? If yes, which one?</t>
+  </si>
+  <si>
+    <t>The buffer used to extract the substance from the sample.</t>
+  </si>
+  <si>
+    <t>The amount of extraction buffer applied.</t>
+  </si>
+  <si>
+    <t>The name of the input (the source) of this assay.</t>
+  </si>
 </sst>
 </file>
 
@@ -401,7 +428,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -441,6 +468,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -487,7 +520,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -594,10 +627,21 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{87CB12D2-5D32-5344-BA63-4377B67E3763}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -667,7 +711,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -983,48 +1027,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5EEB8C5-4C05-AA46-9FA8-0D61FE068A75}">
   <dimension ref="A1:XFB32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="13" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="F24" sqref="F24:F28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="22" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.83203125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="54.6640625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.1640625" style="16" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="57.33203125" style="16" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="37.875" style="15" customWidth="1"/>
+    <col min="3" max="3" width="54.625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="14.625" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.375" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.375" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.125" style="16" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="57.375" style="16" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="29.5" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="58.1640625" style="16" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="64.33203125" style="16" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="37.33203125" style="16" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="48.1640625" style="16" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="54.33203125" style="16" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="29.83203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="58.125" style="16" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="64.375" style="16" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="37.375" style="16" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="48.125" style="16" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="54.375" style="16" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="29.875" style="16" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="58.5" style="16" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="64.6640625" style="16" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="28.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="57.1640625" style="16" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="63.33203125" style="16" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="35.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="64.625" style="16" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="28.375" style="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="57.125" style="16" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="63.375" style="16" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="35.375" style="16" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="64" style="16" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="70.1640625" style="16" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="37.33203125" style="16" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="48.1640625" style="16" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="54.33203125" style="16" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="29.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="58.33203125" style="16" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="70.125" style="16" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="37.375" style="16" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="48.125" style="16" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="54.375" style="16" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="29.625" style="16" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="58.375" style="16" hidden="1" customWidth="1"/>
     <col min="29" max="29" width="64.5" style="16" hidden="1" customWidth="1"/>
-    <col min="30" max="16384" width="10.83203125" style="16"/>
+    <col min="30" max="16384" width="10.875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>61</v>
       </c>
@@ -1059,7 +1103,7 @@
       <c r="AB1" s="4"/>
       <c r="AC1" s="2"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>61</v>
       </c>
@@ -1144,7 +1188,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>61</v>
       </c>
@@ -1177,7 +1221,7 @@
       <c r="AB3"/>
       <c r="AC3"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -1208,7 +1252,7 @@
       <c r="AB4" s="17"/>
       <c r="AC4" s="17"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>63</v>
       </c>
@@ -1251,7 +1295,7 @@
       <c r="AB5" s="18"/>
       <c r="AC5" s="18"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>63</v>
       </c>
@@ -1292,7 +1336,7 @@
       <c r="AB6" s="18"/>
       <c r="AC6" s="18"/>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>63</v>
       </c>
@@ -1327,7 +1371,7 @@
       <c r="AB7" s="18"/>
       <c r="AC7" s="18"/>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>63</v>
       </c>
@@ -1362,7 +1406,7 @@
       <c r="AB8" s="18"/>
       <c r="AC8" s="18"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>63</v>
       </c>
@@ -1395,7 +1439,7 @@
       <c r="AB9" s="18"/>
       <c r="AC9" s="18"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>63</v>
       </c>
@@ -1428,7 +1472,7 @@
       <c r="AB10" s="18"/>
       <c r="AC10" s="18"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -1459,7 +1503,7 @@
       <c r="AB11" s="17"/>
       <c r="AC11" s="17"/>
     </row>
-    <row r="12" spans="1:29" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>64</v>
       </c>
@@ -1508,7 +1552,7 @@
       <c r="AB12" s="19"/>
       <c r="AC12" s="19"/>
     </row>
-    <row r="13" spans="1:29" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>64</v>
       </c>
@@ -1557,7 +1601,7 @@
       <c r="AB13" s="20"/>
       <c r="AC13" s="20"/>
     </row>
-    <row r="14" spans="1:29" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>64</v>
       </c>
@@ -1594,7 +1638,7 @@
       <c r="AB14" s="21"/>
       <c r="AC14" s="21"/>
     </row>
-    <row r="15" spans="1:29" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>64</v>
       </c>
@@ -1635,7 +1679,7 @@
       <c r="AB15" s="21"/>
       <c r="AC15" s="21"/>
     </row>
-    <row r="16" spans="1:29" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>70</v>
       </c>
@@ -1645,8 +1689,12 @@
       <c r="C16" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="22"/>
-      <c r="E16" s="21"/>
+      <c r="D16" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" s="46" t="s">
+        <v>97</v>
+      </c>
       <c r="F16" s="21"/>
       <c r="G16" s="21"/>
       <c r="H16" s="21"/>
@@ -1659,10 +1707,14 @@
       <c r="O16" s="21"/>
       <c r="P16" s="22"/>
       <c r="Q16" s="22"/>
-      <c r="R16" s="23"/>
+      <c r="R16" s="49" t="s">
+        <v>100</v>
+      </c>
       <c r="S16" s="23"/>
       <c r="T16" s="23"/>
-      <c r="U16" s="23"/>
+      <c r="U16" s="48" t="s">
+        <v>101</v>
+      </c>
       <c r="V16" s="23"/>
       <c r="W16" s="23"/>
       <c r="X16" s="23"/>
@@ -1672,7 +1724,7 @@
       <c r="AB16" s="22"/>
       <c r="AC16" s="22"/>
     </row>
-    <row r="17" spans="1:16382" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>70</v>
       </c>
@@ -1707,7 +1759,7 @@
       <c r="AB17" s="23"/>
       <c r="AC17" s="23"/>
     </row>
-    <row r="18" spans="1:16382" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>73</v>
       </c>
@@ -1744,7 +1796,7 @@
       <c r="AB18" s="21"/>
       <c r="AC18" s="21"/>
     </row>
-    <row r="19" spans="1:16382" ht="34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>73</v>
       </c>
@@ -1781,7 +1833,7 @@
       <c r="AB19" s="21"/>
       <c r="AC19" s="21"/>
     </row>
-    <row r="20" spans="1:16382" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>73</v>
       </c>
@@ -1820,7 +1872,7 @@
       <c r="AB20" s="21"/>
       <c r="AC20" s="21"/>
     </row>
-    <row r="21" spans="1:16382" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>73</v>
       </c>
@@ -1830,32 +1882,42 @@
       <c r="C21" s="37"/>
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
+      <c r="F21" s="47" t="s">
+        <v>98</v>
+      </c>
       <c r="G21" s="21"/>
       <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
+      <c r="I21" s="47" t="s">
+        <v>98</v>
+      </c>
       <c r="J21" s="21"/>
       <c r="K21" s="21"/>
       <c r="L21" s="21"/>
       <c r="M21" s="21"/>
       <c r="N21" s="21"/>
-      <c r="O21" s="21"/>
+      <c r="O21" s="47" t="s">
+        <v>98</v>
+      </c>
       <c r="P21" s="21"/>
       <c r="Q21" s="21"/>
       <c r="R21" s="21"/>
       <c r="S21" s="21"/>
       <c r="T21" s="21"/>
-      <c r="U21" s="21"/>
+      <c r="U21" s="50" t="s">
+        <v>99</v>
+      </c>
       <c r="V21" s="21"/>
       <c r="W21" s="21"/>
       <c r="X21" s="21"/>
       <c r="Y21" s="21"/>
       <c r="Z21" s="21"/>
-      <c r="AA21" s="21"/>
+      <c r="AA21" s="47" t="s">
+        <v>98</v>
+      </c>
       <c r="AB21" s="21"/>
       <c r="AC21" s="21"/>
     </row>
-    <row r="22" spans="1:16382" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16382" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -1886,7 +1948,7 @@
       <c r="AB22" s="24"/>
       <c r="AC22" s="24"/>
     </row>
-    <row r="23" spans="1:16382" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16382" x14ac:dyDescent="0.25">
       <c r="A23" s="40"/>
       <c r="B23" s="40"/>
       <c r="C23" s="40"/>
@@ -1917,7 +1979,7 @@
       <c r="AB23" s="24"/>
       <c r="AC23" s="24"/>
     </row>
-    <row r="24" spans="1:16382" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16382" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="45" t="s">
         <v>57</v>
       </c>
@@ -1966,7 +2028,7 @@
       <c r="AB24" s="21"/>
       <c r="AC24" s="21"/>
     </row>
-    <row r="25" spans="1:16382" ht="34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16382" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="45" t="s">
         <v>57</v>
       </c>
@@ -2015,7 +2077,7 @@
       <c r="AB25" s="21"/>
       <c r="AC25" s="21"/>
     </row>
-    <row r="26" spans="1:16382" ht="51" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16382" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A26" s="45" t="s">
         <v>57</v>
       </c>
@@ -2064,7 +2126,7 @@
       <c r="AB26" s="21"/>
       <c r="AC26" s="21"/>
     </row>
-    <row r="27" spans="1:16382" ht="51" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16382" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A27" s="45" t="s">
         <v>57</v>
       </c>
@@ -2113,7 +2175,7 @@
       <c r="AB27" s="21"/>
       <c r="AC27" s="21"/>
     </row>
-    <row r="28" spans="1:16382" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16382" x14ac:dyDescent="0.25">
       <c r="A28" s="45" t="s">
         <v>57</v>
       </c>
@@ -2162,7 +2224,7 @@
       <c r="AB28" s="21"/>
       <c r="AC28" s="21"/>
     </row>
-    <row r="29" spans="1:16382" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16382" x14ac:dyDescent="0.25">
       <c r="A29" s="45" t="s">
         <v>57</v>
       </c>
@@ -18552,7 +18614,7 @@
       <c r="XFA29" s="28"/>
       <c r="XFB29" s="28"/>
     </row>
-    <row r="30" spans="1:16382" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16382" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="44"/>
       <c r="B30" s="44"/>
       <c r="C30" s="44"/>
@@ -18583,7 +18645,7 @@
       <c r="AB30" s="29"/>
       <c r="AC30" s="29"/>
     </row>
-    <row r="31" spans="1:16382" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16382" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -34967,7 +35029,7 @@
       <c r="XFA31" s="16"/>
       <c r="XFB31" s="16"/>
     </row>
-    <row r="32" spans="1:16382" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16382" x14ac:dyDescent="0.25">
       <c r="I32" s="26"/>
       <c r="J32" s="26"/>
       <c r="K32" s="26"/>

</xml_diff>

<commit_message>
Update templates to get uploaded via Swobup
</commit_message>
<xml_diff>
--- a/templates/2EXT01_RNA/2EXT01_RNA.xlsx
+++ b/templates/2EXT01_RNA/2EXT01_RNA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\nfdi4plants\SWATE_templates\templates\2EXT01_RNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDC9B7E-89E2-49D8-A7D9-C4472F5C5A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94206B08-20E8-4542-BDB4-5C4530E69ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
   </bookViews>
@@ -1007,7 +1007,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
+  <wetp:taskpane dockstate="right" visibility="0" width="646" row="1">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1031,7 +1031,7 @@
       <pane xSplit="3" ySplit="22" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fix RNA extraction template error
</commit_message>
<xml_diff>
--- a/templates/2EXT01_RNA/2EXT01_RNA.xlsx
+++ b/templates/2EXT01_RNA/2EXT01_RNA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\nfdi4plants\SWATE_templates\templates\2EXT01_RNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94206B08-20E8-4542-BDB4-5C4530E69ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EDAEEC-025D-45D3-ACCB-0F6D3EBC8F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
   </bookViews>
   <sheets>
     <sheet name="2EXT01_RNA" sheetId="3" r:id="rId1"/>
@@ -1007,7 +1007,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="646" row="1">
+  <wetp:taskpane dockstate="right" visibility="0" width="589" row="1">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1028,10 +1028,10 @@
   <dimension ref="A1:XFB32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="22" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="22" topLeftCell="E23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -35065,21 +35065,22 @@
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <customXml>
   <SwateTable Table="annotationTable1" Worksheet="2EXT01_RNA">
-    <TableValidation DateTime="2021-03-12 14:48" SwateVersion="0.4.0" TableName="annotationTable1" Userlist="" WorksheetName="2EXT01_RNA">
+    <TableValidation DateTime="2021-08-09 09:57" SwateVersion="0.4.7" TableName="annotationTable1" Userlist="" WorksheetName="2EXT01_RNA">
       <ColumnValidation ColumnAdress="0" ColumnHeader="Source Name" Importance="None" Unit="None" ValidationFormat="None"/>
       <ColumnValidation ColumnAdress="1" ColumnHeader="Sample Name" Importance="None" Unit="None" ValidationFormat="None"/>
       <ColumnValidation ColumnAdress="2" ColumnHeader="Parameter [Bio entity]" Importance="4" Unit="None" ValidationFormat="OntologyTerm Bio entity"/>
       <ColumnValidation ColumnAdress="5" ColumnHeader="Parameter [Biosource amount]" Importance="4" Unit="milligram" ValidationFormat="UnitTerm milligram"/>
-      <ColumnValidation ColumnAdress="11" ColumnHeader="Parameter [Extraction Kit]" Importance="4" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="11" ColumnHeader="Parameter [Extraction method]" Importance="None" Unit="None" ValidationFormat="None"/>
       <ColumnValidation ColumnAdress="14" ColumnHeader="Parameter [Extraction buffer]" Importance="4" Unit="None" ValidationFormat="None"/>
       <ColumnValidation ColumnAdress="17" ColumnHeader="Parameter [Extraction buffer volume]" Importance="4" Unit="microliter" ValidationFormat="UnitTerm microliter"/>
+      <ColumnValidation ColumnAdress="23" ColumnHeader="Parameter [RNA quality check]" Importance="None" Unit="None" ValidationFormat="None"/>
     </TableValidation>
   </SwateTable>
 </customXml>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C44CF77C-EAFF-5141-BDAC-352B7E3BD96E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78E1A287-D36C-44F2-81B0-ACF9A3896B90}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
some edits to geo related templates
</commit_message>
<xml_diff>
--- a/templates/2EXT01_RNA/2EXT01_RNA.xlsx
+++ b/templates/2EXT01_RNA/2EXT01_RNA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\nfdi4plants\SWATE_templates\templates\2EXT01_RNA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Google Drive/CEPLAS/MetadataTemplates/SWATE_templates/templates/2EXT01_RNA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EDAEEC-025D-45D3-ACCB-0F6D3EBC8F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5414CFEB-A2A4-344F-8D00-3A79F6C181C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
+    <workbookView xWindow="-24600" yWindow="-20880" windowWidth="35760" windowHeight="18640" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
   </bookViews>
   <sheets>
     <sheet name="2EXT01_RNA" sheetId="3" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="106">
   <si>
     <t>Source Name</t>
   </si>
@@ -334,12 +325,6 @@
     <t>The name of the output of this assay</t>
   </si>
   <si>
-    <t>User instruction missing</t>
-  </si>
-  <si>
-    <t>Do we want to give a unit? If yes, which one?</t>
-  </si>
-  <si>
     <t>The buffer used to extract the substance from the sample.</t>
   </si>
   <si>
@@ -347,6 +332,21 @@
   </si>
   <si>
     <t>The name of the input (the source) of this assay.</t>
+  </si>
+  <si>
+    <t>Unit: Microliter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name the method used for extraction (e.g. title and literature reference or commercial kit) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fill the name and / or result of the method used to check the RNA quality. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The amount of material (e.g. plant tissue) used during extraction. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name the biological molecule extracted and measured in this assay. </t>
   </si>
 </sst>
 </file>
@@ -520,7 +520,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -635,13 +635,12 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{87CB12D2-5D32-5344-BA63-4377B67E3763}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -711,7 +710,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1007,7 +1006,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="589" row="1">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="1">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1028,47 +1027,47 @@
   <dimension ref="A1:XFB32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="22" topLeftCell="E23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="22" topLeftCell="I23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.875" style="15" customWidth="1"/>
-    <col min="3" max="3" width="54.625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="14.625" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.375" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.375" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.125" style="16" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="57.375" style="16" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="29.5" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="58.125" style="16" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="64.375" style="16" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="37.375" style="16" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="48.125" style="16" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="54.375" style="16" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="29.875" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.83203125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="54.6640625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="154.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.1640625" style="16" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="57.33203125" style="16" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="69.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="58.1640625" style="16" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="64.33203125" style="16" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="37.33203125" style="16" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="48.1640625" style="16" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="54.33203125" style="16" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="78" style="16" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="58.5" style="16" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="64.625" style="16" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="28.375" style="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="57.125" style="16" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="63.375" style="16" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="35.375" style="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="64.6640625" style="16" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="69.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="57.1640625" style="16" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="63.33203125" style="16" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="69.6640625" style="16" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="64" style="16" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="70.125" style="16" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="37.375" style="16" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="48.125" style="16" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="54.375" style="16" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="29.625" style="16" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="58.375" style="16" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="70.1640625" style="16" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="37.33203125" style="16" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="48.1640625" style="16" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="54.33203125" style="16" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="69.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="58.33203125" style="16" hidden="1" customWidth="1"/>
     <col min="29" max="29" width="64.5" style="16" hidden="1" customWidth="1"/>
-    <col min="30" max="16384" width="10.875" style="16"/>
+    <col min="30" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>61</v>
       </c>
@@ -1103,7 +1102,7 @@
       <c r="AB1" s="4"/>
       <c r="AC1" s="2"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>61</v>
       </c>
@@ -1188,7 +1187,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>61</v>
       </c>
@@ -1221,7 +1220,7 @@
       <c r="AB3"/>
       <c r="AC3"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -1252,7 +1251,7 @@
       <c r="AB4" s="17"/>
       <c r="AC4" s="17"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>63</v>
       </c>
@@ -1295,7 +1294,7 @@
       <c r="AB5" s="18"/>
       <c r="AC5" s="18"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>63</v>
       </c>
@@ -1336,7 +1335,7 @@
       <c r="AB6" s="18"/>
       <c r="AC6" s="18"/>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>63</v>
       </c>
@@ -1371,7 +1370,7 @@
       <c r="AB7" s="18"/>
       <c r="AC7" s="18"/>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>63</v>
       </c>
@@ -1406,7 +1405,7 @@
       <c r="AB8" s="18"/>
       <c r="AC8" s="18"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>63</v>
       </c>
@@ -1439,7 +1438,7 @@
       <c r="AB9" s="18"/>
       <c r="AC9" s="18"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>63</v>
       </c>
@@ -1472,7 +1471,7 @@
       <c r="AB10" s="18"/>
       <c r="AC10" s="18"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -1503,7 +1502,7 @@
       <c r="AB11" s="17"/>
       <c r="AC11" s="17"/>
     </row>
-    <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>64</v>
       </c>
@@ -1552,7 +1551,7 @@
       <c r="AB12" s="19"/>
       <c r="AC12" s="19"/>
     </row>
-    <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>64</v>
       </c>
@@ -1601,7 +1600,7 @@
       <c r="AB13" s="20"/>
       <c r="AC13" s="20"/>
     </row>
-    <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>64</v>
       </c>
@@ -1638,7 +1637,7 @@
       <c r="AB14" s="21"/>
       <c r="AC14" s="21"/>
     </row>
-    <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>64</v>
       </c>
@@ -1669,7 +1668,9 @@
       <c r="R15" s="21"/>
       <c r="S15" s="21"/>
       <c r="T15" s="21"/>
-      <c r="U15" s="21"/>
+      <c r="U15" s="21" t="s">
+        <v>101</v>
+      </c>
       <c r="V15" s="21"/>
       <c r="W15" s="21"/>
       <c r="X15" s="21"/>
@@ -1679,7 +1680,7 @@
       <c r="AB15" s="21"/>
       <c r="AC15" s="21"/>
     </row>
-    <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>70</v>
       </c>
@@ -1690,41 +1691,49 @@
         <v>71</v>
       </c>
       <c r="D16" s="46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E16" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
-      <c r="O16" s="21"/>
+      <c r="F16" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="47" t="s">
+        <v>102</v>
+      </c>
       <c r="P16" s="22"/>
       <c r="Q16" s="22"/>
       <c r="R16" s="49" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="S16" s="23"/>
       <c r="T16" s="23"/>
       <c r="U16" s="48" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="V16" s="23"/>
       <c r="W16" s="23"/>
       <c r="X16" s="23"/>
       <c r="Y16" s="23"/>
       <c r="Z16" s="23"/>
-      <c r="AA16" s="23"/>
+      <c r="AA16" s="48" t="s">
+        <v>103</v>
+      </c>
       <c r="AB16" s="22"/>
       <c r="AC16" s="22"/>
     </row>
-    <row r="17" spans="1:16382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>70</v>
       </c>
@@ -1759,7 +1768,7 @@
       <c r="AB17" s="23"/>
       <c r="AC17" s="23"/>
     </row>
-    <row r="18" spans="1:16382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>73</v>
       </c>
@@ -1796,7 +1805,7 @@
       <c r="AB18" s="21"/>
       <c r="AC18" s="21"/>
     </row>
-    <row r="19" spans="1:16382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>73</v>
       </c>
@@ -1833,7 +1842,7 @@
       <c r="AB19" s="21"/>
       <c r="AC19" s="21"/>
     </row>
-    <row r="20" spans="1:16382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>73</v>
       </c>
@@ -1872,7 +1881,7 @@
       <c r="AB20" s="21"/>
       <c r="AC20" s="21"/>
     </row>
-    <row r="21" spans="1:16382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>73</v>
       </c>
@@ -1882,42 +1891,32 @@
       <c r="C21" s="37"/>
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
-      <c r="F21" s="47" t="s">
-        <v>98</v>
-      </c>
+      <c r="F21" s="21"/>
       <c r="G21" s="21"/>
       <c r="H21" s="21"/>
-      <c r="I21" s="47" t="s">
-        <v>98</v>
-      </c>
+      <c r="I21" s="21"/>
       <c r="J21" s="21"/>
       <c r="K21" s="21"/>
       <c r="L21" s="21"/>
       <c r="M21" s="21"/>
       <c r="N21" s="21"/>
-      <c r="O21" s="47" t="s">
-        <v>98</v>
-      </c>
+      <c r="O21" s="21"/>
       <c r="P21" s="21"/>
       <c r="Q21" s="21"/>
-      <c r="R21" s="21"/>
-      <c r="S21" s="21"/>
-      <c r="T21" s="21"/>
-      <c r="U21" s="50" t="s">
-        <v>99</v>
-      </c>
-      <c r="V21" s="21"/>
-      <c r="W21" s="21"/>
-      <c r="X21" s="21"/>
-      <c r="Y21" s="21"/>
-      <c r="Z21" s="21"/>
-      <c r="AA21" s="47" t="s">
-        <v>98</v>
-      </c>
+      <c r="R21" s="23"/>
+      <c r="S21" s="23"/>
+      <c r="T21" s="23"/>
+      <c r="U21" s="23"/>
+      <c r="V21" s="23"/>
+      <c r="W21" s="23"/>
+      <c r="X21" s="23"/>
+      <c r="Y21" s="23"/>
+      <c r="Z21" s="23"/>
+      <c r="AA21" s="23"/>
       <c r="AB21" s="21"/>
       <c r="AC21" s="21"/>
     </row>
-    <row r="22" spans="1:16382" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16382" x14ac:dyDescent="0.2">
       <c r="A22" s="14"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -1948,7 +1947,7 @@
       <c r="AB22" s="24"/>
       <c r="AC22" s="24"/>
     </row>
-    <row r="23" spans="1:16382" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16382" x14ac:dyDescent="0.2">
       <c r="A23" s="40"/>
       <c r="B23" s="40"/>
       <c r="C23" s="40"/>
@@ -1979,7 +1978,7 @@
       <c r="AB23" s="24"/>
       <c r="AC23" s="24"/>
     </row>
-    <row r="24" spans="1:16382" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16382" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="45" t="s">
         <v>57</v>
       </c>
@@ -2028,7 +2027,7 @@
       <c r="AB24" s="21"/>
       <c r="AC24" s="21"/>
     </row>
-    <row r="25" spans="1:16382" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16382" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="45" t="s">
         <v>57</v>
       </c>
@@ -2040,7 +2039,7 @@
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
-      <c r="F25" t="s">
+      <c r="F25" s="50" t="s">
         <v>93</v>
       </c>
       <c r="G25"/>
@@ -2077,7 +2076,7 @@
       <c r="AB25" s="21"/>
       <c r="AC25" s="21"/>
     </row>
-    <row r="26" spans="1:16382" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16382" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="45" t="s">
         <v>57</v>
       </c>
@@ -2126,7 +2125,7 @@
       <c r="AB26" s="21"/>
       <c r="AC26" s="21"/>
     </row>
-    <row r="27" spans="1:16382" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16382" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="45" t="s">
         <v>57</v>
       </c>
@@ -2138,7 +2137,7 @@
       </c>
       <c r="D27" s="21"/>
       <c r="E27" s="21"/>
-      <c r="F27" t="s">
+      <c r="F27" s="51" t="s">
         <v>95</v>
       </c>
       <c r="G27"/>
@@ -2175,7 +2174,7 @@
       <c r="AB27" s="21"/>
       <c r="AC27" s="21"/>
     </row>
-    <row r="28" spans="1:16382" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16382" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="45" t="s">
         <v>57</v>
       </c>
@@ -2224,7 +2223,7 @@
       <c r="AB28" s="21"/>
       <c r="AC28" s="21"/>
     </row>
-    <row r="29" spans="1:16382" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16382" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="45" t="s">
         <v>57</v>
       </c>
@@ -18614,7 +18613,7 @@
       <c r="XFA29" s="28"/>
       <c r="XFB29" s="28"/>
     </row>
-    <row r="30" spans="1:16382" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16382" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="44"/>
       <c r="B30" s="44"/>
       <c r="C30" s="44"/>
@@ -18645,7 +18644,7 @@
       <c r="AB30" s="29"/>
       <c r="AC30" s="29"/>
     </row>
-    <row r="31" spans="1:16382" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16382" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="15"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -35029,7 +35028,7 @@
       <c r="XFA31" s="16"/>
       <c r="XFB31" s="16"/>
     </row>
-    <row r="32" spans="1:16382" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16382" x14ac:dyDescent="0.2">
       <c r="I32" s="26"/>
       <c r="J32" s="26"/>
       <c r="K32" s="26"/>

</xml_diff>

<commit_message>
minor edits / comments and aligned semantics with NFDI4PSO
</commit_message>
<xml_diff>
--- a/templates/2EXT01_RNA/2EXT01_RNA.xlsx
+++ b/templates/2EXT01_RNA/2EXT01_RNA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Google Drive/CEPLAS/MetadataTemplates/SWATE_templates/templates/2EXT01_RNA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9C514B-7D8B-8343-AFEB-6B07CA63D8CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B8C237-AE6B-5244-BF80-4535B537D199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="500" windowWidth="27900" windowHeight="17500" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="105">
   <si>
     <t>Source Name</t>
   </si>
@@ -310,9 +310,6 @@
     <t>cv</t>
   </si>
   <si>
-    <t>Include one of the following: total RNA, polyA RNA, cytoplasmic RNA, nuclear RNA, genomic DNA, protein, or other.</t>
-  </si>
-  <si>
     <t>The buffer used to extract the substance from the sample.</t>
   </si>
   <si>
@@ -436,7 +433,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -485,6 +482,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -529,7 +532,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -656,6 +659,7 @@
     <xf numFmtId="49" fontId="10" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1047,10 +1051,10 @@
   <dimension ref="A1:XFB34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="24" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="24" topLeftCell="F25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="B31" sqref="B31"/>
+      <selection pane="bottomRight" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1093,7 +1097,7 @@
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="52" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="4"/>
@@ -1689,7 +1693,7 @@
       <c r="S15" s="21"/>
       <c r="T15" s="21"/>
       <c r="U15" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="V15" s="21"/>
       <c r="W15" s="21"/>
@@ -1713,12 +1717,12 @@
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
       <c r="F16" s="46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G16" s="46"/>
       <c r="H16" s="46"/>
       <c r="I16" s="46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J16" s="46"/>
       <c r="K16" s="46"/>
@@ -1726,17 +1730,17 @@
       <c r="M16" s="46"/>
       <c r="N16" s="46"/>
       <c r="O16" s="46" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P16" s="22"/>
       <c r="Q16" s="22"/>
       <c r="R16" s="48" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="S16" s="23"/>
       <c r="T16" s="23"/>
       <c r="U16" s="47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="V16" s="23"/>
       <c r="W16" s="23"/>
@@ -1744,7 +1748,7 @@
       <c r="Y16" s="23"/>
       <c r="Z16" s="23"/>
       <c r="AA16" s="47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AB16" s="22"/>
       <c r="AC16" s="22"/>
@@ -1863,10 +1867,10 @@
         <v>70</v>
       </c>
       <c r="B20" s="49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C20" s="36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D20" s="50"/>
       <c r="E20" s="50"/>
@@ -2000,10 +2004,10 @@
         <v>70</v>
       </c>
       <c r="B21" s="49" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D21" s="50"/>
       <c r="E21" s="50"/>
@@ -2423,7 +2427,7 @@
       </c>
       <c r="D29" s="21"/>
       <c r="E29" s="21"/>
-      <c r="F29" s="21" t="s">
+      <c r="F29" s="54" t="s">
         <v>92</v>
       </c>
       <c r="G29"/>
@@ -2465,16 +2469,14 @@
         <v>56</v>
       </c>
       <c r="B30" s="35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C30" s="36" t="s">
         <v>83</v>
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="21"/>
-      <c r="F30" s="21" t="s">
-        <v>93</v>
-      </c>
+      <c r="F30" s="21"/>
       <c r="G30"/>
       <c r="H30"/>
       <c r="I30" t="s">

</xml_diff>

<commit_message>
Update all (but one) template for technical reasons
</commit_message>
<xml_diff>
--- a/templates/2EXT01_RNA/2EXT01_RNA.xlsx
+++ b/templates/2EXT01_RNA/2EXT01_RNA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Google Drive/CEPLAS/MetadataTemplates/SWATE_templates/templates/2EXT01_RNA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\nfdi4plants\SWATE_templates\templates\2EXT01_RNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F211A66E-523A-9A4B-87C2-C4FD59602564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489E7FB8-189C-4A4E-8795-4721AEAB2B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4720" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
   </bookViews>
   <sheets>
     <sheet name="2EXT01_RNA" sheetId="3" r:id="rId1"/>
@@ -491,9 +491,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="2" builtinId="8"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{87CB12D2-5D32-5344-BA63-4377B67E3763}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -886,40 +886,40 @@
       <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.83203125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="14.625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.375" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="154.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.1640625" style="11" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="57.33203125" style="11" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="69.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="58.1640625" style="11" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="64.33203125" style="11" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="37.33203125" style="11" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="48.1640625" style="11" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="54.33203125" style="11" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="51.125" style="11" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="57.375" style="11" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="69.625" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="58.125" style="11" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="64.375" style="11" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="37.375" style="11" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="48.125" style="11" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="54.375" style="11" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="78" style="11" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="58.5" style="11" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="64.6640625" style="11" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="69.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="57.1640625" style="11" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="63.33203125" style="11" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="69.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="64.625" style="11" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="69.625" style="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="57.125" style="11" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="63.375" style="11" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="69.625" style="11" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="64" style="11" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="70.1640625" style="11" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="37.33203125" style="11" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="48.1640625" style="11" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="54.33203125" style="11" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="69.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="58.33203125" style="11" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="70.125" style="11" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="37.375" style="11" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="48.125" style="11" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="54.375" style="11" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="69.625" style="11" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="58.375" style="11" hidden="1" customWidth="1"/>
     <col min="28" max="28" width="64.5" style="11" hidden="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.83203125" style="11"/>
+    <col min="29" max="16384" width="10.875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>44</v>
       </c>
@@ -953,7 +953,7 @@
       <c r="AA1" s="4"/>
       <c r="AB1" s="2"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>44</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>44</v>
       </c>
@@ -1069,7 +1069,7 @@
       <c r="AA3"/>
       <c r="AB3"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="12"/>
@@ -1099,7 +1099,7 @@
       <c r="AA4" s="12"/>
       <c r="AB4" s="12"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>45</v>
       </c>
@@ -1141,7 +1141,7 @@
       <c r="AA5" s="13"/>
       <c r="AB5" s="13"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>45</v>
       </c>
@@ -1181,7 +1181,7 @@
       <c r="AA6" s="13"/>
       <c r="AB6" s="13"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>45</v>
       </c>
@@ -1215,7 +1215,7 @@
       <c r="AA7" s="13"/>
       <c r="AB7" s="13"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>45</v>
       </c>
@@ -1249,7 +1249,7 @@
       <c r="AA8" s="13"/>
       <c r="AB8" s="13"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>45</v>
       </c>
@@ -1281,7 +1281,7 @@
       <c r="AA9" s="13"/>
       <c r="AB9" s="13"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>45</v>
       </c>
@@ -1313,7 +1313,7 @@
       <c r="AA10" s="13"/>
       <c r="AB10" s="13"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="12"/>
@@ -1343,7 +1343,7 @@
       <c r="AA11" s="12"/>
       <c r="AB11" s="12"/>
     </row>
-    <row r="12" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
         <v>61</v>
       </c>
@@ -1377,7 +1377,7 @@
       <c r="AA12" s="14"/>
       <c r="AB12" s="14"/>
     </row>
-    <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>62</v>
       </c>
@@ -1417,7 +1417,7 @@
       <c r="AA13" s="14"/>
       <c r="AB13" s="14"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
       <c r="B14" s="22"/>
       <c r="C14" s="15"/>
@@ -1447,7 +1447,7 @@
       <c r="AA14" s="15"/>
       <c r="AB14" s="15"/>
     </row>
-    <row r="15" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>41</v>
       </c>
@@ -1493,7 +1493,7 @@
       <c r="AA15" s="14"/>
       <c r="AB15" s="14"/>
     </row>
-    <row r="16" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
         <v>41</v>
       </c>
@@ -1539,7 +1539,7 @@
       <c r="AA16" s="14"/>
       <c r="AB16" s="14"/>
     </row>
-    <row r="17" spans="1:16381" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16381" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
         <v>41</v>
       </c>
@@ -1585,7 +1585,7 @@
       <c r="AA17" s="14"/>
       <c r="AB17" s="14"/>
     </row>
-    <row r="18" spans="1:16381" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16381" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
         <v>41</v>
       </c>
@@ -1631,7 +1631,7 @@
       <c r="AA18" s="14"/>
       <c r="AB18" s="14"/>
     </row>
-    <row r="19" spans="1:16381" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16381" x14ac:dyDescent="0.25">
       <c r="A19" s="26" t="s">
         <v>41</v>
       </c>
@@ -1675,7 +1675,7 @@
       <c r="AA19" s="14"/>
       <c r="AB19" s="14"/>
     </row>
-    <row r="20" spans="1:16381" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16381" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
         <v>41</v>
       </c>
@@ -18062,7 +18062,7 @@
       <c r="XEZ20" s="19"/>
       <c r="XFA20" s="19"/>
     </row>
-    <row r="21" spans="1:16381" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16381" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25"/>
       <c r="B21" s="25"/>
       <c r="C21" s="20"/>
@@ -18092,7 +18092,7 @@
       <c r="AA21" s="20"/>
       <c r="AB21" s="20"/>
     </row>
-    <row r="22" spans="1:16381" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16381" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
@@ -34475,7 +34475,7 @@
       <c r="XEZ22" s="11"/>
       <c r="XFA22" s="11"/>
     </row>
-    <row r="23" spans="1:16381" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16381" x14ac:dyDescent="0.25">
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
       <c r="J23" s="17"/>

</xml_diff>

<commit_message>
Fill empty ER sheets into every template (except Imaging)
</commit_message>
<xml_diff>
--- a/templates/2EXT01_RNA/2EXT01_RNA.xlsx
+++ b/templates/2EXT01_RNA/2EXT01_RNA.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\omaus\SWATE_templates\templates\2EXT01_RNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0078519-3568-45AA-A6AD-D77836331C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E73D29F-AE4C-45D5-A379-EA714AFC3E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2EXT01_RNA" sheetId="1" r:id="rId1"/>
     <sheet name="SwateTemplateMetadata" sheetId="2" r:id="rId2"/>
+    <sheet name="GEO_RNASEQ" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="89">
   <si>
     <t>Source Name</t>
   </si>
@@ -238,6 +239,81 @@
   </si>
   <si>
     <t>1.1.3</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>TermSourceRef</t>
+  </si>
+  <si>
+    <t>Ontology</t>
+  </si>
+  <si>
+    <t>TAN</t>
+  </si>
+  <si>
+    <t>Content type (validation)</t>
+  </si>
+  <si>
+    <t>Notes during templating</t>
+  </si>
+  <si>
+    <t>Target term</t>
+  </si>
+  <si>
+    <t>Instruction</t>
+  </si>
+  <si>
+    <t>Requirement (m/o/n)</t>
+  </si>
+  <si>
+    <t>Value (cv/s/d)</t>
+  </si>
+  <si>
+    <t>Additional information</t>
+  </si>
+  <si>
+    <t>Review comments</t>
+  </si>
+  <si>
+    <t>NFDI4PSO:0000012</t>
+  </si>
+  <si>
+    <t>NFDI4PSO</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000012</t>
+  </si>
+  <si>
+    <t>NFDI4PSO:0000013</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000013</t>
+  </si>
+  <si>
+    <t>NFDI4PSO:0000054</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000054</t>
+  </si>
+  <si>
+    <t>NFDI4PSO:0000050</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000050</t>
+  </si>
+  <si>
+    <t>NFDI4PSO:0000051</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000051</t>
+  </si>
+  <si>
+    <t>NFDI4PSO:0000062</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000062</t>
   </si>
 </sst>
 </file>
@@ -813,7 +889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1170,6 +1246,377 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:L9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K4" t="s">
+        <v>64</v>
+      </c>
+      <c r="L4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I5" t="s">
+        <v>64</v>
+      </c>
+      <c r="J5" t="s">
+        <v>64</v>
+      </c>
+      <c r="K5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J6" t="s">
+        <v>64</v>
+      </c>
+      <c r="K6" t="s">
+        <v>64</v>
+      </c>
+      <c r="L6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" t="s">
+        <v>64</v>
+      </c>
+      <c r="J7" t="s">
+        <v>64</v>
+      </c>
+      <c r="K7" t="s">
+        <v>64</v>
+      </c>
+      <c r="L7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I8" t="s">
+        <v>64</v>
+      </c>
+      <c r="J8" t="s">
+        <v>64</v>
+      </c>
+      <c r="K8" t="s">
+        <v>64</v>
+      </c>
+      <c r="L8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" t="s">
+        <v>64</v>
+      </c>
+      <c r="J9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K9" t="s">
+        <v>64</v>
+      </c>
+      <c r="L9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <customXml>
   <SwateTable Table="annotationTableGoodDingo21">

</xml_diff>

<commit_message>
Fill ER sheets of templates (except Image)
</commit_message>
<xml_diff>
--- a/templates/2EXT01_RNA/2EXT01_RNA.xlsx
+++ b/templates/2EXT01_RNA/2EXT01_RNA.xlsx
@@ -8,19 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\omaus\SWATE_templates\templates\2EXT01_RNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E73D29F-AE4C-45D5-A379-EA714AFC3E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171D4B4E-F308-490C-BF80-C4C6DE898D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2EXT01_RNA" sheetId="1" r:id="rId1"/>
     <sheet name="SwateTemplateMetadata" sheetId="2" r:id="rId2"/>
     <sheet name="GEO_RNASEQ" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -47,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="100">
   <si>
     <t>Source Name</t>
   </si>
@@ -314,6 +323,39 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000062</t>
+  </si>
+  <si>
+    <t>Unit: microgram</t>
+  </si>
+  <si>
+    <t>Unit: Microliter</t>
+  </si>
+  <si>
+    <t>SAMPLES_molecule</t>
+  </si>
+  <si>
+    <t>Type of molecule that was extracted from the biological material. Include one of the following: total RNA, polyA RNA, cytoplasmic RNA, nuclear RNA, genomic DNA, protein, or other.</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>cv</t>
+  </si>
+  <si>
+    <t>PROTOCOLS_extract protocol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Describe the protocols used to extract and prepare the material to be sequenced. </t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>at least some info is required, but not all terms</t>
   </si>
 </sst>
 </file>
@@ -373,7 +415,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -451,11 +493,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD2D2D2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD2D2D2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD2D2D2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD2D2D2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -488,6 +545,12 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -889,7 +952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1250,9 +1313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1262,7 +1323,7 @@
     <col min="4" max="4" width="46.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
@@ -1271,344 +1332,296 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="13" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="G2" t="s">
+      <c r="C3" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="H2" t="s">
+      <c r="D3" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="I2" t="s">
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="J2" t="s">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="K2" t="s">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="L5" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="L2" t="s">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="L6" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="L7" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="L8" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I3" t="s">
-        <v>64</v>
-      </c>
-      <c r="J3" t="s">
-        <v>64</v>
-      </c>
-      <c r="K3" t="s">
-        <v>64</v>
-      </c>
-      <c r="L3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="D4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" t="s">
-        <v>64</v>
-      </c>
-      <c r="G4" t="s">
-        <v>64</v>
-      </c>
-      <c r="H4" t="s">
-        <v>64</v>
-      </c>
-      <c r="I4" t="s">
-        <v>64</v>
-      </c>
-      <c r="J4" t="s">
-        <v>64</v>
-      </c>
-      <c r="K4" t="s">
-        <v>64</v>
-      </c>
-      <c r="L4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I5" t="s">
-        <v>64</v>
-      </c>
-      <c r="J5" t="s">
-        <v>64</v>
-      </c>
-      <c r="K5" t="s">
-        <v>64</v>
-      </c>
-      <c r="L5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" t="s">
-        <v>64</v>
-      </c>
-      <c r="G6" t="s">
-        <v>64</v>
-      </c>
-      <c r="H6" t="s">
-        <v>64</v>
-      </c>
-      <c r="I6" t="s">
-        <v>64</v>
-      </c>
-      <c r="J6" t="s">
-        <v>64</v>
-      </c>
-      <c r="K6" t="s">
-        <v>64</v>
-      </c>
-      <c r="L6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" t="s">
-        <v>64</v>
-      </c>
-      <c r="G7" t="s">
-        <v>64</v>
-      </c>
-      <c r="H7" t="s">
-        <v>64</v>
-      </c>
-      <c r="I7" t="s">
-        <v>64</v>
-      </c>
-      <c r="J7" t="s">
-        <v>64</v>
-      </c>
-      <c r="K7" t="s">
-        <v>64</v>
-      </c>
-      <c r="L7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G8" t="s">
-        <v>64</v>
-      </c>
-      <c r="H8" t="s">
-        <v>64</v>
-      </c>
-      <c r="I8" t="s">
-        <v>64</v>
-      </c>
-      <c r="J8" t="s">
-        <v>64</v>
-      </c>
-      <c r="K8" t="s">
-        <v>64</v>
-      </c>
-      <c r="L8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C9" t="s">
-        <v>77</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="D9" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="E9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" t="s">
-        <v>64</v>
-      </c>
-      <c r="G9" t="s">
-        <v>64</v>
-      </c>
-      <c r="H9" t="s">
-        <v>64</v>
-      </c>
-      <c r="I9" t="s">
-        <v>64</v>
-      </c>
-      <c r="J9" t="s">
-        <v>64</v>
-      </c>
-      <c r="K9" t="s">
-        <v>64</v>
-      </c>
-      <c r="L9" t="s">
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="L9" s="14" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add content examples from old templates, add checklist
</commit_message>
<xml_diff>
--- a/templates/2EXT01_RNA/2EXT01_RNA.xlsx
+++ b/templates/2EXT01_RNA/2EXT01_RNA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\omaus\SWATE_templates\templates\2EXT01_RNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171D4B4E-F308-490C-BF80-C4C6DE898D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84163D4-8D24-4B64-A6BE-2BC697C2093A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="110">
   <si>
     <t>Source Name</t>
   </si>
@@ -247,9 +247,6 @@
     <t>Dominik</t>
   </si>
   <si>
-    <t>1.1.3</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -356,6 +353,39 @@
   </si>
   <si>
     <t>at least some info is required, but not all terms</t>
+  </si>
+  <si>
+    <t>RNA (Transcriptomics)</t>
+  </si>
+  <si>
+    <t>DNA (Genomics)</t>
+  </si>
+  <si>
+    <t>Metabolites</t>
+  </si>
+  <si>
+    <t>Protein</t>
+  </si>
+  <si>
+    <t>QIAGEN RNEasy</t>
+  </si>
+  <si>
+    <t>PCI method</t>
+  </si>
+  <si>
+    <t>QIAGEN RNEasy Buffer 2</t>
+  </si>
+  <si>
+    <t>phenol:chloroform:isopropanol</t>
+  </si>
+  <si>
+    <t>RIN: 8.1</t>
+  </si>
+  <si>
+    <t>RNA quality checked by PAGE</t>
+  </si>
+  <si>
+    <t>1.1.4</t>
   </si>
 </sst>
 </file>
@@ -366,7 +396,7 @@
     <numFmt numFmtId="164" formatCode="0.00\ &quot;milligram&quot;"/>
     <numFmt numFmtId="165" formatCode="0.00\ &quot;microliter&quot;"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,6 +408,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFF5F5F5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -509,8 +546,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -553,7 +591,8 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{F5E1E0D5-7FB4-4F22-8D3C-EFCDC257DFA2}"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
@@ -628,8 +667,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B4158286-A58C-485B-8494-948292CED1F3}" name="annotationTableGoodDingo21" displayName="annotationTableGoodDingo21" ref="A1:V2" totalsRowShown="0">
-  <autoFilter ref="A1:V2" xr:uid="{B4158286-A58C-485B-8494-948292CED1F3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B4158286-A58C-485B-8494-948292CED1F3}" name="annotationTableGoodDingo21" displayName="annotationTableGoodDingo21" ref="A1:V5" totalsRowShown="0">
+  <autoFilter ref="A1:V5" xr:uid="{B4158286-A58C-485B-8494-948292CED1F3}"/>
   <tableColumns count="22">
     <tableColumn id="1" xr3:uid="{DF71AA61-E923-4AAC-A8BA-9D46DCD4BAC1}" name="Source Name"/>
     <tableColumn id="3" xr3:uid="{17F12197-5A6B-46DB-84FA-86D856A5419D}" name="Parameter [Bio entity]"/>
@@ -935,6 +974,9 @@
   <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
+  <wetp:taskpane dockstate="right" visibility="0" width="662" row="2">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+  </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
@@ -948,9 +990,19 @@
 </we:webextension>
 </file>
 
+<file path=xl/webextensions/webextension2.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{37A029A9-1C46-4A69-B4EA-D70C9D760220}">
+  <we:reference id="5d6f5462-3401-48ec-9406-d12882e9ad84" version="0.5.1.0" store="\\DT-P-2020-04-OM\swate_manifests" storeType="Filesystem"/>
+  <we:alternateReferences/>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1049,23 +1101,106 @@
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>99</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="L2" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
-      <c r="O2" s="2"/>
+      <c r="O2" s="2">
+        <v>200</v>
+      </c>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
+      <c r="S2" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1108,7 +1243,7 @@
         <v>24</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>63</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1333,40 +1468,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>74</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1374,13 +1509,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
@@ -1390,7 +1525,7 @@
       <c r="J2" s="14"/>
       <c r="K2" s="14"/>
       <c r="L2" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1398,13 +1533,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
@@ -1414,7 +1549,7 @@
       <c r="J3" s="14"/>
       <c r="K3" s="14"/>
       <c r="L3" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1422,33 +1557,33 @@
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="D4" s="14" t="s">
         <v>77</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>78</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G4" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="I4" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="J4" s="14" t="s">
         <v>93</v>
-      </c>
-      <c r="J4" s="14" t="s">
-        <v>94</v>
       </c>
       <c r="K4" s="14"/>
       <c r="L4" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1456,35 +1591,35 @@
         <v>5</v>
       </c>
       <c r="B5" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="14" t="s">
         <v>79</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>80</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G5" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H5" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="I5" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="J5" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="K5" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="K5" s="14" t="s">
-        <v>99</v>
-      </c>
       <c r="L5" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1492,33 +1627,33 @@
         <v>9</v>
       </c>
       <c r="B6" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="14" t="s">
         <v>81</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>82</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H6" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="I6" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="J6" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="K6" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="K6" s="14" t="s">
-        <v>99</v>
-      </c>
       <c r="L6" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1526,33 +1661,33 @@
         <v>12</v>
       </c>
       <c r="B7" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>83</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>84</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H7" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="I7" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="J7" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="K7" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="K7" s="14" t="s">
-        <v>99</v>
-      </c>
       <c r="L7" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1560,35 +1695,35 @@
         <v>15</v>
       </c>
       <c r="B8" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>85</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>86</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G8" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H8" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="I8" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="J8" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="K8" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="K8" s="14" t="s">
-        <v>99</v>
-      </c>
       <c r="L8" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1596,33 +1731,33 @@
         <v>19</v>
       </c>
       <c r="B9" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>87</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>88</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H9" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="I9" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="J9" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="K9" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="K9" s="14" t="s">
-        <v>99</v>
-      </c>
       <c r="L9" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1633,22 +1768,22 @@
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <customXml>
   <SwateTable Table="annotationTableGoodDingo21">
-    <TableValidation DateTime="2021-11-03 16:47" SwateVersion="0.5.1" TableName="annotationTableGoodDingo21" Userlist="">
-      <ColumnValidation ColumnAdress="0" ColumnHeader="Source Name" Importance="None" Unit="None" ValidationFormat="None"/>
-      <ColumnValidation ColumnAdress="1" ColumnHeader="Parameter [Bio entity]" Importance="None" Unit="None" ValidationFormat="None"/>
-      <ColumnValidation ColumnAdress="4" ColumnHeader="Parameter [Biosource amount]" Importance="None" Unit="None" ValidationFormat="None"/>
+    <TableValidation DateTime="2021-12-13 19:05" SwateVersion="0.5.1" TableName="annotationTableGoodDingo21" Userlist="">
+      <ColumnValidation ColumnAdress="0" ColumnHeader="Source Name" Importance="5" Unit="None" ValidationFormat="Text"/>
+      <ColumnValidation ColumnAdress="1" ColumnHeader="Parameter [Bio entity]" Importance="4" Unit="None" ValidationFormat="OntologyTerm (Bio entity)"/>
+      <ColumnValidation ColumnAdress="4" ColumnHeader="Parameter [Biosource amount]" Importance="4" Unit="None" ValidationFormat="UnitTerm milligram"/>
       <ColumnValidation ColumnAdress="8" ColumnHeader="Parameter [Extraction method]" Importance="None" Unit="None" ValidationFormat="None"/>
-      <ColumnValidation ColumnAdress="11" ColumnHeader="Parameter [Extraction buffer]" Importance="None" Unit="None" ValidationFormat="None"/>
-      <ColumnValidation ColumnAdress="14" ColumnHeader="Parameter [Extraction buffer volume]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="11" ColumnHeader="Parameter [Extraction buffer]" Importance="4" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="14" ColumnHeader="Parameter [Extraction buffer volume]" Importance="4" Unit="None" ValidationFormat="UnitTerm microliter"/>
       <ColumnValidation ColumnAdress="18" ColumnHeader="Parameter [RNA quality check]" Importance="None" Unit="None" ValidationFormat="None"/>
-      <ColumnValidation ColumnAdress="21" ColumnHeader="Sample Name" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="21" ColumnHeader="Sample Name" Importance="5" Unit="None" ValidationFormat="Text"/>
     </TableValidation>
   </SwateTable>
 </customXml>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE06DD7-E578-419D-9372-D72935A33CB2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{598E9532-73B5-45A6-90F3-D9D590F0DD8E}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>